<commit_message>
updated all phonetics models, removed superfluous analysis
</commit_message>
<xml_diff>
--- a/Ch_7_Sentence_Modes/Excel/Utterance and Phonetics LMEMs.xlsx
+++ b/Ch_7_Sentence_Modes/Excel/Utterance and Phonetics LMEMs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Github\PhD\Ch_7_Sentence_Modes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AA4ACB-190C-4B7B-96CF-7DABB6529B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855551D5-15C8-46E8-9B25-7ED954B8D63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
   </bookViews>
@@ -1016,16 +1016,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.5</c:v>
+                    <c:v>-4.16282891543577</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1139999999999999</c:v>
+                    <c:v>-4.2763356740591654</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.228</c:v>
+                    <c:v>-4.1454741533326196</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.214</c:v>
+                    <c:v>-4.3008921454628801</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1037,16 +1037,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>1.5</c:v>
+                    <c:v>-4.16282891543577</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1139999999999999</c:v>
+                    <c:v>-4.2763356740591654</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.228</c:v>
+                    <c:v>-4.1454741533326196</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.214</c:v>
+                    <c:v>-4.3008921454628801</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1089,16 +1089,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-1.694</c:v>
+                  <c:v>-1.9490000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.7210000000000001</c:v>
+                  <c:v>-4.0419999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7</c:v>
+                  <c:v>0.95799999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6859999999999999</c:v>
+                  <c:v>3.121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1499,16 +1499,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.208999999999989</c:v>
+                    <c:v>-3.6105682313773997</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.921999999999997</c:v>
+                    <c:v>-3.2832849483673101</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0889999999999986</c:v>
+                    <c:v>-3.4313201102335995</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.5789999999999935</c:v>
+                    <c:v>-3.7964852688148056</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1520,16 +1520,16 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
                   <c:pt idx="0">
-                    <c:v>2.208999999999989</c:v>
+                    <c:v>-3.6105682313773997</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.921999999999997</c:v>
+                    <c:v>-3.2832849483673101</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.0889999999999986</c:v>
+                    <c:v>-3.4313201102335995</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.5789999999999935</c:v>
+                    <c:v>-3.7964852688148056</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1572,16 +1572,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>89.230999999999995</c:v>
+                  <c:v>86.793999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.652000000000001</c:v>
+                  <c:v>87.263999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.016999999999996</c:v>
+                  <c:v>87.325999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91.546999999999997</c:v>
+                  <c:v>88.405000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2491,13 +2491,13 @@
             <v>estimate</v>
           </cell>
           <cell r="C1" t="str">
+            <v>conf.low</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>conf.high</v>
+          </cell>
+          <cell r="E1" t="str">
             <v>std.error</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>2.5% CI</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>97.5% CI</v>
           </cell>
           <cell r="F1" t="str">
             <v>z.value</v>
@@ -2520,28 +2520,28 @@
             <v>modeMDC</v>
           </cell>
           <cell r="B2">
-            <v>89.230999999999995</v>
+            <v>86.793999999999997</v>
           </cell>
           <cell r="C2">
-            <v>1.127</v>
+            <v>83.183735333271997</v>
           </cell>
           <cell r="D2">
-            <v>87.022000000000006</v>
+            <v>90.404568231377397</v>
           </cell>
           <cell r="E2">
-            <v>91.44</v>
+            <v>1.6619999999999999</v>
           </cell>
           <cell r="F2">
-            <v>79.168999999999997</v>
+            <v>52.21</v>
           </cell>
           <cell r="G2">
-            <v>11.69</v>
+            <v>12.36</v>
           </cell>
           <cell r="H2">
-            <v>2.5500000000000001E-17</v>
+            <v>7.1E-16</v>
           </cell>
           <cell r="I2">
-            <v>2.0400000000000001E-16</v>
+            <v>1.9000000000000001E-15</v>
           </cell>
           <cell r="J2" t="str">
             <v>p&lt;0.0001</v>
@@ -2552,28 +2552,28 @@
             <v>modeMWH</v>
           </cell>
           <cell r="B3">
-            <v>89.652000000000001</v>
+            <v>87.263999999999996</v>
           </cell>
           <cell r="C3">
-            <v>0.98099999999999998</v>
+            <v>83.979921593540197</v>
           </cell>
           <cell r="D3">
-            <v>87.73</v>
+            <v>90.547284948367306</v>
           </cell>
           <cell r="E3">
-            <v>91.573999999999998</v>
+            <v>1.5129999999999999</v>
           </cell>
           <cell r="F3">
-            <v>91.424999999999997</v>
+            <v>57.667000000000002</v>
           </cell>
           <cell r="G3">
-            <v>10.119999999999999</v>
+            <v>12.46</v>
           </cell>
           <cell r="H3">
-            <v>4.28E-16</v>
+            <v>1.7E-16</v>
           </cell>
           <cell r="I3">
-            <v>2.57E-15</v>
+            <v>1.3E-15</v>
           </cell>
           <cell r="J3" t="str">
             <v>p&lt;0.0001</v>
@@ -2584,28 +2584,28 @@
             <v>modeMYN</v>
           </cell>
           <cell r="B4">
-            <v>90.016999999999996</v>
+            <v>87.325999999999993</v>
           </cell>
           <cell r="C4">
-            <v>1.0660000000000001</v>
+            <v>83.895222032976804</v>
           </cell>
           <cell r="D4">
-            <v>87.927999999999997</v>
+            <v>90.757320110233593</v>
           </cell>
           <cell r="E4">
-            <v>92.106999999999999</v>
+            <v>1.58</v>
           </cell>
           <cell r="F4">
-            <v>84.435000000000002</v>
+            <v>55.283000000000001</v>
           </cell>
           <cell r="G4">
-            <v>11.53</v>
+            <v>12.35</v>
           </cell>
           <cell r="H4">
-            <v>1.86E-17</v>
+            <v>3.5999999999999998E-16</v>
           </cell>
           <cell r="I4">
-            <v>2.0400000000000001E-16</v>
+            <v>1.4999999999999999E-15</v>
           </cell>
           <cell r="J4" t="str">
             <v>p&lt;0.0001</v>
@@ -2616,28 +2616,28 @@
             <v>modeMDQ</v>
           </cell>
           <cell r="B5">
-            <v>91.546999999999997</v>
+            <v>88.405000000000001</v>
           </cell>
           <cell r="C5">
-            <v>1.3160000000000001</v>
+            <v>84.609277983035</v>
           </cell>
           <cell r="D5">
-            <v>88.968000000000004</v>
+            <v>92.201485268814807</v>
           </cell>
           <cell r="E5">
-            <v>94.126000000000005</v>
+            <v>1.7450000000000001</v>
           </cell>
           <cell r="F5">
-            <v>69.561999999999998</v>
+            <v>50.655999999999999</v>
           </cell>
           <cell r="G5">
-            <v>12.73</v>
+            <v>12.19</v>
           </cell>
           <cell r="H5">
-            <v>8.2800000000000006E-18</v>
+            <v>1.4999999999999999E-15</v>
           </cell>
           <cell r="I5">
-            <v>1.99E-16</v>
+            <v>2.9999999999999998E-15</v>
           </cell>
           <cell r="J5" t="str">
             <v>p&lt;0.0001</v>
@@ -2665,13 +2665,13 @@
             <v>estimate</v>
           </cell>
           <cell r="C1" t="str">
+            <v>conf.low</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>conf.high</v>
+          </cell>
+          <cell r="E1" t="str">
             <v>std.error</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>2.5% CI</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>97.5% CI</v>
           </cell>
           <cell r="F1" t="str">
             <v>z.value</v>
@@ -2691,115 +2691,109 @@
         </row>
         <row r="2">
           <cell r="B2">
-            <v>-1.694</v>
+            <v>-1.9490000000000001</v>
           </cell>
           <cell r="C2">
-            <v>0.76500000000000001</v>
+            <v>-6.1117594117146599</v>
           </cell>
           <cell r="D2">
-            <v>-3.194</v>
+            <v>2.2138289154357702</v>
           </cell>
           <cell r="E2">
-            <v>-0.19400000000000001</v>
+            <v>1.86</v>
           </cell>
           <cell r="F2">
-            <v>-2.2130000000000001</v>
+            <v>-1.048</v>
           </cell>
           <cell r="G2">
-            <v>13.41</v>
+            <v>9.69</v>
           </cell>
           <cell r="H2">
-            <v>4.48E-2</v>
+            <v>0.32</v>
           </cell>
           <cell r="I2">
-            <v>5.3800000000000001E-2</v>
+            <v>0.36599999999999999</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>-3.7210000000000001</v>
+            <v>-4.0419999999999998</v>
           </cell>
           <cell r="C3">
-            <v>1.0780000000000001</v>
+            <v>-8.3184683304519602</v>
           </cell>
           <cell r="D3">
-            <v>-5.835</v>
+            <v>0.234335674059166</v>
           </cell>
           <cell r="E3">
-            <v>-1.6080000000000001</v>
+            <v>1.95</v>
           </cell>
           <cell r="F3">
-            <v>-3.4510000000000001</v>
+            <v>-2.073</v>
           </cell>
           <cell r="G3">
-            <v>9.61</v>
+            <v>11.34</v>
           </cell>
           <cell r="H3">
-            <v>6.6E-3</v>
+            <v>6.2E-2</v>
           </cell>
           <cell r="I3">
-            <v>1.18E-2</v>
+            <v>9.9000000000000005E-2</v>
           </cell>
           <cell r="J3" t="str">
-            <v>p&lt;0.05</v>
+            <v>(p&lt;0.1)</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>1.7</v>
+            <v>0.95799999999999996</v>
           </cell>
           <cell r="C4">
-            <v>0.627</v>
+            <v>-3.18785071466518</v>
           </cell>
           <cell r="D4">
-            <v>0.47199999999999998</v>
+            <v>5.1034741533326198</v>
           </cell>
           <cell r="E4">
-            <v>2.9289999999999998</v>
+            <v>1.8420000000000001</v>
           </cell>
           <cell r="F4">
-            <v>2.7130000000000001</v>
+            <v>0.52</v>
           </cell>
           <cell r="G4">
-            <v>10.58</v>
+            <v>9.33</v>
           </cell>
           <cell r="H4">
-            <v>2.0799999999999999E-2</v>
+            <v>0.61499999999999999</v>
           </cell>
           <cell r="I4">
-            <v>2.7799999999999998E-2</v>
-          </cell>
-          <cell r="J4" t="str">
-            <v>p&lt;0.05</v>
+            <v>0.61499999999999999</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5">
-            <v>4.6859999999999999</v>
+            <v>3.121</v>
           </cell>
           <cell r="C5">
-            <v>1.129</v>
+            <v>-1.1798261362714799</v>
           </cell>
           <cell r="D5">
-            <v>2.472</v>
+            <v>7.4218921454628797</v>
           </cell>
           <cell r="E5">
-            <v>6.899</v>
+            <v>1.966</v>
           </cell>
           <cell r="F5">
-            <v>4.149</v>
+            <v>1.5880000000000001</v>
           </cell>
           <cell r="G5">
-            <v>12.74</v>
+            <v>11.56</v>
           </cell>
           <cell r="H5">
-            <v>1.1999999999999999E-3</v>
+            <v>0.13900000000000001</v>
           </cell>
           <cell r="I5">
-            <v>2.8999999999999998E-3</v>
-          </cell>
-          <cell r="J5" t="str">
-            <v>p&lt;0.01</v>
+            <v>0.186</v>
           </cell>
         </row>
       </sheetData>
@@ -2827,13 +2821,13 @@
             <v>estimate</v>
           </cell>
           <cell r="D1" t="str">
+            <v>conf.low</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>conf.high</v>
+          </cell>
+          <cell r="F1" t="str">
             <v>std.error</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>2.5% CI</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>97.5% CI</v>
           </cell>
           <cell r="G1" t="str">
             <v>z.value</v>
@@ -2859,28 +2853,28 @@
             <v>modeMWH</v>
           </cell>
           <cell r="C2">
-            <v>0.42099999999999999</v>
+            <v>0.46899999999999997</v>
           </cell>
           <cell r="D2">
-            <v>0.312</v>
+            <v>-0.22800809788462301</v>
           </cell>
           <cell r="E2">
-            <v>-0.191</v>
+            <v>1.16691223729475</v>
           </cell>
           <cell r="F2">
-            <v>1.0329999999999999</v>
+            <v>0.313</v>
           </cell>
           <cell r="G2">
-            <v>1.349</v>
+            <v>1.4990000000000001</v>
           </cell>
           <cell r="H2">
-            <v>10.8</v>
+            <v>10.06</v>
           </cell>
           <cell r="I2">
-            <v>0.2051</v>
+            <v>0.16500000000000001</v>
           </cell>
           <cell r="J2">
-            <v>0.214</v>
+            <v>0.17799999999999999</v>
           </cell>
         </row>
         <row r="3">
@@ -2891,28 +2885,28 @@
             <v>modeMYN</v>
           </cell>
           <cell r="C3">
-            <v>0.78600000000000003</v>
+            <v>0.53200000000000003</v>
           </cell>
           <cell r="D3">
-            <v>0.25</v>
+            <v>7.3813273986569797E-2</v>
           </cell>
           <cell r="E3">
-            <v>0.29599999999999999</v>
+            <v>0.99043054836575695</v>
           </cell>
           <cell r="F3">
-            <v>1.2769999999999999</v>
+            <v>0.20699999999999999</v>
           </cell>
           <cell r="G3">
-            <v>3.1419999999999999</v>
+            <v>2.5659999999999998</v>
           </cell>
           <cell r="H3">
-            <v>10.37</v>
+            <v>10.63</v>
           </cell>
           <cell r="I3">
-            <v>0.01</v>
+            <v>2.7E-2</v>
           </cell>
           <cell r="J3">
-            <v>1.5100000000000001E-2</v>
+            <v>4.3999999999999997E-2</v>
           </cell>
           <cell r="K3" t="str">
             <v>p&lt;0.05</v>
@@ -2926,28 +2920,28 @@
             <v>modeMDQ</v>
           </cell>
           <cell r="C4">
-            <v>2.3159999999999998</v>
+            <v>1.611</v>
           </cell>
           <cell r="D4">
-            <v>0.442</v>
+            <v>0.74795525994970802</v>
           </cell>
           <cell r="E4">
-            <v>1.4490000000000001</v>
+            <v>2.4745315263488998</v>
           </cell>
           <cell r="F4">
-            <v>3.1829999999999998</v>
+            <v>0.39300000000000002</v>
           </cell>
           <cell r="G4">
-            <v>5.2370000000000001</v>
+            <v>4.0960000000000001</v>
           </cell>
           <cell r="H4">
-            <v>10.17</v>
+            <v>11.26</v>
           </cell>
           <cell r="I4">
-            <v>3.6000000000000002E-4</v>
+            <v>2E-3</v>
           </cell>
           <cell r="J4">
-            <v>1.1999999999999999E-3</v>
+            <v>5.0000000000000001E-3</v>
           </cell>
           <cell r="K4" t="str">
             <v>p&lt;0.01</v>
@@ -2961,28 +2955,28 @@
             <v>modeMYN</v>
           </cell>
           <cell r="C5">
-            <v>0.36499999999999999</v>
+            <v>6.3E-2</v>
           </cell>
           <cell r="D5">
-            <v>0.26700000000000002</v>
+            <v>-0.47452675858097398</v>
           </cell>
           <cell r="E5">
-            <v>-0.158</v>
+            <v>0.59986469357665495</v>
           </cell>
           <cell r="F5">
-            <v>0.88900000000000001</v>
+            <v>0.24299999999999999</v>
           </cell>
           <cell r="G5">
-            <v>1.3680000000000001</v>
+            <v>0.25800000000000001</v>
           </cell>
           <cell r="H5">
-            <v>12.73</v>
+            <v>10.59</v>
           </cell>
           <cell r="I5">
-            <v>0.1951</v>
+            <v>0.80100000000000005</v>
           </cell>
           <cell r="J5">
-            <v>0.21290000000000001</v>
+            <v>0.80100000000000005</v>
           </cell>
         </row>
         <row r="6">
@@ -2993,31 +2987,28 @@
             <v>modeMDQ</v>
           </cell>
           <cell r="C6">
-            <v>1.8959999999999999</v>
+            <v>1.1419999999999999</v>
           </cell>
           <cell r="D6">
-            <v>0.63900000000000001</v>
+            <v>-0.153117733840856</v>
           </cell>
           <cell r="E6">
-            <v>0.64400000000000002</v>
+            <v>2.4366962216536301</v>
           </cell>
           <cell r="F6">
-            <v>3.1469999999999998</v>
+            <v>0.58499999999999996</v>
           </cell>
           <cell r="G6">
-            <v>2.968</v>
+            <v>1.9510000000000001</v>
           </cell>
           <cell r="H6">
-            <v>10.51</v>
+            <v>10.56</v>
           </cell>
           <cell r="I6">
-            <v>1.34E-2</v>
+            <v>7.8E-2</v>
           </cell>
           <cell r="J6">
-            <v>1.89E-2</v>
-          </cell>
-          <cell r="K6" t="str">
-            <v>p&lt;0.05</v>
+            <v>0.10199999999999999</v>
           </cell>
         </row>
         <row r="7">
@@ -3028,31 +3019,31 @@
             <v>modeMDQ</v>
           </cell>
           <cell r="C7">
-            <v>1.53</v>
+            <v>1.079</v>
           </cell>
           <cell r="D7">
-            <v>0.58799999999999997</v>
+            <v>-4.86078358637431E-2</v>
           </cell>
           <cell r="E7">
-            <v>0.377</v>
+            <v>2.2068583933924799</v>
           </cell>
           <cell r="F7">
-            <v>2.6829999999999998</v>
+            <v>0.50700000000000001</v>
           </cell>
           <cell r="G7">
-            <v>2.6019999999999999</v>
+            <v>2.1269999999999998</v>
           </cell>
           <cell r="H7">
-            <v>10.050000000000001</v>
+            <v>10.17</v>
           </cell>
           <cell r="I7">
-            <v>2.63E-2</v>
+            <v>5.8999999999999997E-2</v>
           </cell>
           <cell r="J7">
-            <v>3.32E-2</v>
+            <v>8.5000000000000006E-2</v>
           </cell>
           <cell r="K7" t="str">
-            <v>p&lt;0.05</v>
+            <v>(p&lt;0.1)</v>
           </cell>
         </row>
       </sheetData>
@@ -3071,12 +3062,12 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0.94231623989217705</v>
+            <v>0.96083371545006302</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.52849012129538697</v>
+            <v>1.2545781673086001E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -3104,13 +3095,13 @@
             <v>estimate</v>
           </cell>
           <cell r="D1" t="str">
+            <v>conf.low</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>conf.high</v>
+          </cell>
+          <cell r="F1" t="str">
             <v>std.error</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>2.5% CI</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>97.5% CI</v>
           </cell>
           <cell r="G1" t="str">
             <v>z.value</v>
@@ -3136,28 +3127,28 @@
             <v>modeMWH</v>
           </cell>
           <cell r="C2">
-            <v>-2.028</v>
+            <v>-2.093</v>
           </cell>
           <cell r="D2">
-            <v>1.234</v>
+            <v>-4.8500048198338899</v>
           </cell>
           <cell r="E2">
-            <v>-4.4470000000000001</v>
+            <v>0.66381613021775598</v>
           </cell>
           <cell r="F2">
-            <v>0.39200000000000002</v>
+            <v>1.2390000000000001</v>
           </cell>
           <cell r="G2">
-            <v>-1.643</v>
+            <v>-1.6890000000000001</v>
           </cell>
           <cell r="H2">
-            <v>10.15</v>
+            <v>10.11</v>
           </cell>
           <cell r="I2">
-            <v>0.13100000000000001</v>
+            <v>0.122</v>
           </cell>
           <cell r="J2">
-            <v>0.14979999999999999</v>
+            <v>0.14399999999999999</v>
           </cell>
         </row>
         <row r="3">
@@ -3168,28 +3159,28 @@
             <v>modeMYN</v>
           </cell>
           <cell r="C3">
-            <v>3.3940000000000001</v>
+            <v>2.907</v>
           </cell>
           <cell r="D3">
-            <v>0.8</v>
+            <v>1.2891062804668101</v>
           </cell>
           <cell r="E3">
-            <v>1.825</v>
+            <v>4.5244332348265397</v>
           </cell>
           <cell r="F3">
-            <v>4.9630000000000001</v>
+            <v>0.72699999999999998</v>
           </cell>
           <cell r="G3">
-            <v>4.24</v>
+            <v>3.9969999999999999</v>
           </cell>
           <cell r="H3">
-            <v>10.02</v>
+            <v>10.119999999999999</v>
           </cell>
           <cell r="I3">
-            <v>1.6999999999999999E-3</v>
+            <v>2E-3</v>
           </cell>
           <cell r="J3">
-            <v>3.7000000000000002E-3</v>
+            <v>6.0000000000000001E-3</v>
           </cell>
           <cell r="K3" t="str">
             <v>p&lt;0.01</v>
@@ -3203,31 +3194,31 @@
             <v>modeMDQ</v>
           </cell>
           <cell r="C4">
-            <v>6.38</v>
+            <v>5.07</v>
           </cell>
           <cell r="D4">
-            <v>1.1180000000000001</v>
+            <v>3.0169488394014401</v>
           </cell>
           <cell r="E4">
-            <v>4.1890000000000001</v>
+            <v>7.1230429774581703</v>
           </cell>
           <cell r="F4">
-            <v>8.57</v>
+            <v>0.93</v>
           </cell>
           <cell r="G4">
-            <v>5.7089999999999996</v>
+            <v>5.4489999999999998</v>
           </cell>
           <cell r="H4">
-            <v>10.119999999999999</v>
+            <v>10.78</v>
           </cell>
           <cell r="I4">
-            <v>1.8699999999999999E-4</v>
+            <v>2.2000000000000001E-4</v>
           </cell>
           <cell r="J4">
-            <v>8.9999999999999998E-4</v>
+            <v>1E-3</v>
           </cell>
           <cell r="K4" t="str">
-            <v>p&lt;0.001</v>
+            <v>p&lt;0.01</v>
           </cell>
         </row>
         <row r="5">
@@ -3238,25 +3229,25 @@
             <v>modeMYN</v>
           </cell>
           <cell r="C5">
-            <v>5.4219999999999997</v>
+            <v>5</v>
           </cell>
           <cell r="D5">
-            <v>1.4370000000000001</v>
+            <v>2.0744151301770501</v>
           </cell>
           <cell r="E5">
-            <v>2.6059999999999999</v>
+            <v>7.9253164313353501</v>
           </cell>
           <cell r="F5">
-            <v>8.2379999999999995</v>
+            <v>1.3169999999999999</v>
           </cell>
           <cell r="G5">
-            <v>3.7730000000000001</v>
+            <v>3.7959999999999998</v>
           </cell>
           <cell r="H5">
-            <v>10.26</v>
+            <v>10.24</v>
           </cell>
           <cell r="I5">
-            <v>3.5000000000000001E-3</v>
+            <v>3.0000000000000001E-3</v>
           </cell>
           <cell r="J5">
             <v>7.0000000000000001E-3</v>
@@ -3273,28 +3264,28 @@
             <v>modeMDQ</v>
           </cell>
           <cell r="C6">
-            <v>8.407</v>
+            <v>7.1630000000000003</v>
           </cell>
           <cell r="D6">
-            <v>1.796</v>
+            <v>3.63149587483408</v>
           </cell>
           <cell r="E6">
-            <v>4.8860000000000001</v>
+            <v>10.694690908964599</v>
           </cell>
           <cell r="F6">
-            <v>11.928000000000001</v>
+            <v>1.593</v>
           </cell>
           <cell r="G6">
-            <v>4.68</v>
+            <v>4.4950000000000001</v>
           </cell>
           <cell r="H6">
-            <v>10.199999999999999</v>
+            <v>10.41</v>
           </cell>
           <cell r="I6">
-            <v>8.2200000000000003E-4</v>
+            <v>1E-3</v>
           </cell>
           <cell r="J6">
-            <v>2.2000000000000001E-3</v>
+            <v>5.0000000000000001E-3</v>
           </cell>
           <cell r="K6" t="str">
             <v>p&lt;0.01</v>
@@ -3308,31 +3299,31 @@
             <v>modeMDQ</v>
           </cell>
           <cell r="C7">
-            <v>2.9849999999999999</v>
+            <v>2.1629999999999998</v>
           </cell>
           <cell r="D7">
-            <v>0.876</v>
+            <v>0.87233269943435898</v>
           </cell>
           <cell r="E7">
-            <v>1.268</v>
+            <v>3.4541186027926698</v>
           </cell>
           <cell r="F7">
-            <v>4.7030000000000003</v>
+            <v>0.57799999999999996</v>
           </cell>
           <cell r="G7">
-            <v>3.4060000000000001</v>
+            <v>3.74</v>
           </cell>
           <cell r="H7">
-            <v>9.83</v>
+            <v>9.8699999999999992</v>
           </cell>
           <cell r="I7">
-            <v>6.8999999999999999E-3</v>
+            <v>4.0000000000000001E-3</v>
           </cell>
           <cell r="J7">
-            <v>1.18E-2</v>
+            <v>7.0000000000000001E-3</v>
           </cell>
           <cell r="K7" t="str">
-            <v>p&lt;0.05</v>
+            <v>p&lt;0.01</v>
           </cell>
         </row>
       </sheetData>
@@ -3351,12 +3342,12 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0.83641134398527495</v>
+            <v>0.91258286194614602</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>0.51029969546325904</v>
+            <v>0.26953753570664701</v>
           </cell>
         </row>
       </sheetData>
@@ -3665,7 +3656,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3714,15 +3705,15 @@
       </c>
       <c r="C2" s="8" t="str">
         <f>[1]utt_f0_b0!C1</f>
-        <v>std.error</v>
+        <v>conf.low</v>
       </c>
       <c r="D2" s="8" t="str">
         <f>[1]utt_f0_b0!D1</f>
-        <v>2.5% CI</v>
+        <v>conf.high</v>
       </c>
       <c r="E2" s="8" t="str">
         <f>[1]utt_f0_b0!E1</f>
-        <v>97.5% CI</v>
+        <v>std.error</v>
       </c>
       <c r="F2" s="8" t="str">
         <f>[1]utt_f0_b0!F1</f>
@@ -3755,35 +3746,35 @@
       </c>
       <c r="B3" s="12">
         <f>[1]utt_f0_b0!B2</f>
-        <v>89.230999999999995</v>
+        <v>86.793999999999997</v>
       </c>
       <c r="C3" s="12">
         <f>[1]utt_f0_b0!C2</f>
-        <v>1.127</v>
+        <v>83.183735333271997</v>
       </c>
       <c r="D3" s="12">
         <f>[1]utt_f0_b0!D2</f>
-        <v>87.022000000000006</v>
+        <v>90.404568231377397</v>
       </c>
       <c r="E3" s="12">
         <f>[1]utt_f0_b0!E2</f>
-        <v>91.44</v>
+        <v>1.6619999999999999</v>
       </c>
       <c r="F3" s="12">
         <f>[1]utt_f0_b0!F2</f>
-        <v>79.168999999999997</v>
+        <v>52.21</v>
       </c>
       <c r="G3" s="12">
         <f>[1]utt_f0_b0!G2</f>
-        <v>11.69</v>
+        <v>12.36</v>
       </c>
       <c r="H3" s="13">
         <f>[1]utt_f0_b0!H2</f>
-        <v>2.5500000000000001E-17</v>
+        <v>7.1E-16</v>
       </c>
       <c r="I3" s="13">
         <f>[1]utt_f0_b0!I2</f>
-        <v>2.0400000000000001E-16</v>
+        <v>1.9000000000000001E-15</v>
       </c>
       <c r="J3" s="14" t="str">
         <f>[1]utt_f0_b0!J2</f>
@@ -3791,7 +3782,7 @@
       </c>
       <c r="K3" s="12">
         <f>B3-D3</f>
-        <v>2.208999999999989</v>
+        <v>-3.6105682313773997</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3801,35 +3792,35 @@
       </c>
       <c r="B4" s="17">
         <f>[1]utt_f0_b0!B3</f>
-        <v>89.652000000000001</v>
+        <v>87.263999999999996</v>
       </c>
       <c r="C4" s="17">
         <f>[1]utt_f0_b0!C3</f>
-        <v>0.98099999999999998</v>
+        <v>83.979921593540197</v>
       </c>
       <c r="D4" s="17">
         <f>[1]utt_f0_b0!D3</f>
-        <v>87.73</v>
+        <v>90.547284948367306</v>
       </c>
       <c r="E4" s="17">
         <f>[1]utt_f0_b0!E3</f>
-        <v>91.573999999999998</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="F4" s="17">
         <f>[1]utt_f0_b0!F3</f>
-        <v>91.424999999999997</v>
+        <v>57.667000000000002</v>
       </c>
       <c r="G4" s="17">
         <f>[1]utt_f0_b0!G3</f>
-        <v>10.119999999999999</v>
+        <v>12.46</v>
       </c>
       <c r="H4" s="18">
         <f>[1]utt_f0_b0!H3</f>
-        <v>4.28E-16</v>
+        <v>1.7E-16</v>
       </c>
       <c r="I4" s="18">
         <f>[1]utt_f0_b0!I3</f>
-        <v>2.57E-15</v>
+        <v>1.3E-15</v>
       </c>
       <c r="J4" s="19" t="str">
         <f>[1]utt_f0_b0!J3</f>
@@ -3837,7 +3828,7 @@
       </c>
       <c r="K4" s="17">
         <f t="shared" ref="K4:K6" si="0">B4-D4</f>
-        <v>1.921999999999997</v>
+        <v>-3.2832849483673101</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3847,35 +3838,35 @@
       </c>
       <c r="B5" s="17">
         <f>[1]utt_f0_b0!B4</f>
-        <v>90.016999999999996</v>
+        <v>87.325999999999993</v>
       </c>
       <c r="C5" s="17">
         <f>[1]utt_f0_b0!C4</f>
-        <v>1.0660000000000001</v>
+        <v>83.895222032976804</v>
       </c>
       <c r="D5" s="17">
         <f>[1]utt_f0_b0!D4</f>
-        <v>87.927999999999997</v>
+        <v>90.757320110233593</v>
       </c>
       <c r="E5" s="17">
         <f>[1]utt_f0_b0!E4</f>
-        <v>92.106999999999999</v>
+        <v>1.58</v>
       </c>
       <c r="F5" s="17">
         <f>[1]utt_f0_b0!F4</f>
-        <v>84.435000000000002</v>
+        <v>55.283000000000001</v>
       </c>
       <c r="G5" s="17">
         <f>[1]utt_f0_b0!G4</f>
-        <v>11.53</v>
+        <v>12.35</v>
       </c>
       <c r="H5" s="18">
         <f>[1]utt_f0_b0!H4</f>
-        <v>1.86E-17</v>
+        <v>3.5999999999999998E-16</v>
       </c>
       <c r="I5" s="18">
         <f>[1]utt_f0_b0!I4</f>
-        <v>2.0400000000000001E-16</v>
+        <v>1.4999999999999999E-15</v>
       </c>
       <c r="J5" s="19" t="str">
         <f>[1]utt_f0_b0!J4</f>
@@ -3883,7 +3874,7 @@
       </c>
       <c r="K5" s="17">
         <f t="shared" si="0"/>
-        <v>2.0889999999999986</v>
+        <v>-3.4313201102335995</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3893,35 +3884,35 @@
       </c>
       <c r="B6" s="21">
         <f>[1]utt_f0_b0!B5</f>
-        <v>91.546999999999997</v>
+        <v>88.405000000000001</v>
       </c>
       <c r="C6" s="21">
         <f>[1]utt_f0_b0!C5</f>
-        <v>1.3160000000000001</v>
+        <v>84.609277983035</v>
       </c>
       <c r="D6" s="21">
         <f>[1]utt_f0_b0!D5</f>
-        <v>88.968000000000004</v>
+        <v>92.201485268814807</v>
       </c>
       <c r="E6" s="21">
         <f>[1]utt_f0_b0!E5</f>
-        <v>94.126000000000005</v>
+        <v>1.7450000000000001</v>
       </c>
       <c r="F6" s="21">
         <f>[1]utt_f0_b0!F5</f>
-        <v>69.561999999999998</v>
+        <v>50.655999999999999</v>
       </c>
       <c r="G6" s="21">
         <f>[1]utt_f0_b0!G5</f>
-        <v>12.73</v>
+        <v>12.19</v>
       </c>
       <c r="H6" s="22">
         <f>[1]utt_f0_b0!H5</f>
-        <v>8.2800000000000006E-18</v>
+        <v>1.4999999999999999E-15</v>
       </c>
       <c r="I6" s="22">
         <f>[1]utt_f0_b0!I5</f>
-        <v>1.99E-16</v>
+        <v>2.9999999999999998E-15</v>
       </c>
       <c r="J6" s="23" t="str">
         <f>[1]utt_f0_b0!J5</f>
@@ -3929,7 +3920,7 @@
       </c>
       <c r="K6" s="21">
         <f t="shared" si="0"/>
-        <v>2.5789999999999935</v>
+        <v>-3.7964852688148056</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3971,15 +3962,15 @@
       </c>
       <c r="C9" s="8" t="str">
         <f>[2]utt_slope_b0!C1</f>
-        <v>std.error</v>
+        <v>conf.low</v>
       </c>
       <c r="D9" s="8" t="str">
         <f>[2]utt_slope_b0!D1</f>
-        <v>2.5% CI</v>
+        <v>conf.high</v>
       </c>
       <c r="E9" s="8" t="str">
         <f>[2]utt_slope_b0!E1</f>
-        <v>97.5% CI</v>
+        <v>std.error</v>
       </c>
       <c r="F9" s="8" t="str">
         <f>[2]utt_slope_b0!F1</f>
@@ -4011,35 +4002,35 @@
       </c>
       <c r="B10" s="12">
         <f>[2]utt_slope_b0!B2</f>
-        <v>-1.694</v>
+        <v>-1.9490000000000001</v>
       </c>
       <c r="C10" s="12">
         <f>[2]utt_slope_b0!C2</f>
-        <v>0.76500000000000001</v>
+        <v>-6.1117594117146599</v>
       </c>
       <c r="D10" s="12">
         <f>[2]utt_slope_b0!D2</f>
-        <v>-3.194</v>
+        <v>2.2138289154357702</v>
       </c>
       <c r="E10" s="12">
         <f>[2]utt_slope_b0!E2</f>
-        <v>-0.19400000000000001</v>
+        <v>1.86</v>
       </c>
       <c r="F10" s="12">
         <f>[2]utt_slope_b0!F2</f>
-        <v>-2.2130000000000001</v>
+        <v>-1.048</v>
       </c>
       <c r="G10" s="12">
         <f>[2]utt_slope_b0!G2</f>
-        <v>13.41</v>
+        <v>9.69</v>
       </c>
       <c r="H10" s="13">
         <f>[2]utt_slope_b0!H2</f>
-        <v>4.48E-2</v>
+        <v>0.32</v>
       </c>
       <c r="I10" s="13">
         <f>[2]utt_slope_b0!I2</f>
-        <v>5.3800000000000001E-2</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="J10" s="14">
         <f>[2]utt_slope_b0!J2</f>
@@ -4047,7 +4038,7 @@
       </c>
       <c r="K10" s="12">
         <f>B10-D10</f>
-        <v>1.5</v>
+        <v>-4.16282891543577</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4056,43 +4047,43 @@
       </c>
       <c r="B11" s="17">
         <f>[2]utt_slope_b0!B3</f>
-        <v>-3.7210000000000001</v>
+        <v>-4.0419999999999998</v>
       </c>
       <c r="C11" s="17">
         <f>[2]utt_slope_b0!C3</f>
-        <v>1.0780000000000001</v>
+        <v>-8.3184683304519602</v>
       </c>
       <c r="D11" s="17">
         <f>[2]utt_slope_b0!D3</f>
-        <v>-5.835</v>
+        <v>0.234335674059166</v>
       </c>
       <c r="E11" s="17">
         <f>[2]utt_slope_b0!E3</f>
-        <v>-1.6080000000000001</v>
+        <v>1.95</v>
       </c>
       <c r="F11" s="17">
         <f>[2]utt_slope_b0!F3</f>
-        <v>-3.4510000000000001</v>
+        <v>-2.073</v>
       </c>
       <c r="G11" s="17">
         <f>[2]utt_slope_b0!G3</f>
-        <v>9.61</v>
+        <v>11.34</v>
       </c>
       <c r="H11" s="18">
         <f>[2]utt_slope_b0!H3</f>
-        <v>6.6E-3</v>
+        <v>6.2E-2</v>
       </c>
       <c r="I11" s="18">
         <f>[2]utt_slope_b0!I3</f>
-        <v>1.18E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="J11" s="19" t="str">
         <f>[2]utt_slope_b0!J3</f>
-        <v>p&lt;0.05</v>
+        <v>(p&lt;0.1)</v>
       </c>
       <c r="K11" s="17">
         <f t="shared" ref="K11:K13" si="1">B11-D11</f>
-        <v>2.1139999999999999</v>
+        <v>-4.2763356740591654</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4101,43 +4092,43 @@
       </c>
       <c r="B12" s="17">
         <f>[2]utt_slope_b0!B4</f>
-        <v>1.7</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="C12" s="17">
         <f>[2]utt_slope_b0!C4</f>
-        <v>0.627</v>
+        <v>-3.18785071466518</v>
       </c>
       <c r="D12" s="17">
         <f>[2]utt_slope_b0!D4</f>
-        <v>0.47199999999999998</v>
+        <v>5.1034741533326198</v>
       </c>
       <c r="E12" s="17">
         <f>[2]utt_slope_b0!E4</f>
-        <v>2.9289999999999998</v>
+        <v>1.8420000000000001</v>
       </c>
       <c r="F12" s="17">
         <f>[2]utt_slope_b0!F4</f>
-        <v>2.7130000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="G12" s="17">
         <f>[2]utt_slope_b0!G4</f>
-        <v>10.58</v>
+        <v>9.33</v>
       </c>
       <c r="H12" s="18">
         <f>[2]utt_slope_b0!H4</f>
-        <v>2.0799999999999999E-2</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="I12" s="18">
         <f>[2]utt_slope_b0!I4</f>
-        <v>2.7799999999999998E-2</v>
-      </c>
-      <c r="J12" s="19" t="str">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="J12" s="19">
         <f>[2]utt_slope_b0!J4</f>
-        <v>p&lt;0.05</v>
+        <v>0</v>
       </c>
       <c r="K12" s="17">
         <f t="shared" si="1"/>
-        <v>1.228</v>
+        <v>-4.1454741533326196</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="15" customFormat="1" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4146,43 +4137,43 @@
       </c>
       <c r="B13" s="21">
         <f>[2]utt_slope_b0!B5</f>
-        <v>4.6859999999999999</v>
+        <v>3.121</v>
       </c>
       <c r="C13" s="21">
         <f>[2]utt_slope_b0!C5</f>
-        <v>1.129</v>
+        <v>-1.1798261362714799</v>
       </c>
       <c r="D13" s="21">
         <f>[2]utt_slope_b0!D5</f>
-        <v>2.472</v>
+        <v>7.4218921454628797</v>
       </c>
       <c r="E13" s="21">
         <f>[2]utt_slope_b0!E5</f>
-        <v>6.899</v>
+        <v>1.966</v>
       </c>
       <c r="F13" s="21">
         <f>[2]utt_slope_b0!F5</f>
-        <v>4.149</v>
+        <v>1.5880000000000001</v>
       </c>
       <c r="G13" s="21">
         <f>[2]utt_slope_b0!G5</f>
-        <v>12.74</v>
+        <v>11.56</v>
       </c>
       <c r="H13" s="22">
         <f>[2]utt_slope_b0!H5</f>
-        <v>1.1999999999999999E-3</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="I13" s="22">
         <f>[2]utt_slope_b0!I5</f>
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="J13" s="23" t="str">
+        <v>0.186</v>
+      </c>
+      <c r="J13" s="23">
         <f>[2]utt_slope_b0!J5</f>
-        <v>p&lt;0.01</v>
+        <v>0</v>
       </c>
       <c r="K13" s="21">
         <f t="shared" si="1"/>
-        <v>2.214</v>
+        <v>-4.3008921454628801</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4424,15 +4415,15 @@
       </c>
       <c r="D2" s="8" t="str">
         <f>[3]utt_f0_b1!D1</f>
-        <v>std.error</v>
+        <v>conf.low</v>
       </c>
       <c r="E2" s="8" t="str">
         <f>[3]utt_f0_b1!E1</f>
-        <v>2.5% CI</v>
+        <v>conf.high</v>
       </c>
       <c r="F2" s="8" t="str">
         <f>[3]utt_f0_b1!F1</f>
-        <v>97.5% CI</v>
+        <v>std.error</v>
       </c>
       <c r="G2" s="8" t="str">
         <f>[3]utt_f0_b1!G1</f>
@@ -4472,35 +4463,35 @@
       </c>
       <c r="C3" s="12">
         <f>[3]utt_f0_b1!C2</f>
-        <v>0.42099999999999999</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="D3" s="12">
         <f>[3]utt_f0_b1!D2</f>
-        <v>0.312</v>
+        <v>-0.22800809788462301</v>
       </c>
       <c r="E3" s="12">
         <f>[3]utt_f0_b1!E2</f>
-        <v>-0.191</v>
+        <v>1.16691223729475</v>
       </c>
       <c r="F3" s="12">
         <f>[3]utt_f0_b1!F2</f>
-        <v>1.0329999999999999</v>
+        <v>0.313</v>
       </c>
       <c r="G3" s="12">
         <f>[3]utt_f0_b1!G2</f>
-        <v>1.349</v>
+        <v>1.4990000000000001</v>
       </c>
       <c r="H3" s="13">
         <f>[3]utt_f0_b1!H2</f>
-        <v>10.8</v>
+        <v>10.06</v>
       </c>
       <c r="I3" s="13">
         <f>[3]utt_f0_b1!I2</f>
-        <v>0.2051</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="J3" s="38">
         <f>[3]utt_f0_b1!J2</f>
-        <v>0.214</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="K3" s="11">
         <f>[3]utt_f0_b1!K2</f>
@@ -4508,11 +4499,11 @@
       </c>
       <c r="M3" s="39">
         <f>[4]utt_f0_r2!$B$3</f>
-        <v>0.52849012129538697</v>
+        <v>1.2545781673086001E-2</v>
       </c>
       <c r="N3" s="39">
         <f>[4]utt_f0_r2!$B$2</f>
-        <v>0.94231623989217705</v>
+        <v>0.96083371545006302</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4526,35 +4517,35 @@
       </c>
       <c r="C4" s="17">
         <f>[3]utt_f0_b1!C3</f>
-        <v>0.78600000000000003</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="D4" s="17">
         <f>[3]utt_f0_b1!D3</f>
-        <v>0.25</v>
+        <v>7.3813273986569797E-2</v>
       </c>
       <c r="E4" s="17">
         <f>[3]utt_f0_b1!E3</f>
-        <v>0.29599999999999999</v>
+        <v>0.99043054836575695</v>
       </c>
       <c r="F4" s="17">
         <f>[3]utt_f0_b1!F3</f>
-        <v>1.2769999999999999</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="G4" s="17">
         <f>[3]utt_f0_b1!G3</f>
-        <v>3.1419999999999999</v>
+        <v>2.5659999999999998</v>
       </c>
       <c r="H4" s="18">
         <f>[3]utt_f0_b1!H3</f>
-        <v>10.37</v>
+        <v>10.63</v>
       </c>
       <c r="I4" s="18">
         <f>[3]utt_f0_b1!I3</f>
-        <v>0.01</v>
+        <v>2.7E-2</v>
       </c>
       <c r="J4" s="40">
         <f>[3]utt_f0_b1!J3</f>
-        <v>1.5100000000000001E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="K4" s="16" t="str">
         <f>[3]utt_f0_b1!K3</f>
@@ -4572,35 +4563,35 @@
       </c>
       <c r="C5" s="17">
         <f>[3]utt_f0_b1!C4</f>
-        <v>2.3159999999999998</v>
+        <v>1.611</v>
       </c>
       <c r="D5" s="17">
         <f>[3]utt_f0_b1!D4</f>
-        <v>0.442</v>
+        <v>0.74795525994970802</v>
       </c>
       <c r="E5" s="17">
         <f>[3]utt_f0_b1!E4</f>
-        <v>1.4490000000000001</v>
+        <v>2.4745315263488998</v>
       </c>
       <c r="F5" s="17">
         <f>[3]utt_f0_b1!F4</f>
-        <v>3.1829999999999998</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="G5" s="17">
         <f>[3]utt_f0_b1!G4</f>
-        <v>5.2370000000000001</v>
+        <v>4.0960000000000001</v>
       </c>
       <c r="H5" s="18">
         <f>[3]utt_f0_b1!H4</f>
-        <v>10.17</v>
+        <v>11.26</v>
       </c>
       <c r="I5" s="18">
         <f>[3]utt_f0_b1!I4</f>
-        <v>3.6000000000000002E-4</v>
+        <v>2E-3</v>
       </c>
       <c r="J5" s="40">
         <f>[3]utt_f0_b1!J4</f>
-        <v>1.1999999999999999E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K5" s="16" t="str">
         <f>[3]utt_f0_b1!K4</f>
@@ -4618,35 +4609,35 @@
       </c>
       <c r="C6" s="17">
         <f>[3]utt_f0_b1!C5</f>
-        <v>0.36499999999999999</v>
+        <v>6.3E-2</v>
       </c>
       <c r="D6" s="17">
         <f>[3]utt_f0_b1!D5</f>
-        <v>0.26700000000000002</v>
+        <v>-0.47452675858097398</v>
       </c>
       <c r="E6" s="17">
         <f>[3]utt_f0_b1!E5</f>
-        <v>-0.158</v>
+        <v>0.59986469357665495</v>
       </c>
       <c r="F6" s="17">
         <f>[3]utt_f0_b1!F5</f>
-        <v>0.88900000000000001</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="G6" s="17">
         <f>[3]utt_f0_b1!G5</f>
-        <v>1.3680000000000001</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="H6" s="18">
         <f>[3]utt_f0_b1!H5</f>
-        <v>12.73</v>
+        <v>10.59</v>
       </c>
       <c r="I6" s="18">
         <f>[3]utt_f0_b1!I5</f>
-        <v>0.1951</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="J6" s="40">
         <f>[3]utt_f0_b1!J5</f>
-        <v>0.21290000000000001</v>
+        <v>0.80100000000000005</v>
       </c>
       <c r="K6" s="16">
         <f>[3]utt_f0_b1!K5</f>
@@ -4664,39 +4655,39 @@
       </c>
       <c r="C7" s="17">
         <f>[3]utt_f0_b1!C6</f>
-        <v>1.8959999999999999</v>
+        <v>1.1419999999999999</v>
       </c>
       <c r="D7" s="17">
         <f>[3]utt_f0_b1!D6</f>
-        <v>0.63900000000000001</v>
+        <v>-0.153117733840856</v>
       </c>
       <c r="E7" s="17">
         <f>[3]utt_f0_b1!E6</f>
-        <v>0.64400000000000002</v>
+        <v>2.4366962216536301</v>
       </c>
       <c r="F7" s="17">
         <f>[3]utt_f0_b1!F6</f>
-        <v>3.1469999999999998</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="G7" s="17">
         <f>[3]utt_f0_b1!G6</f>
-        <v>2.968</v>
+        <v>1.9510000000000001</v>
       </c>
       <c r="H7" s="18">
         <f>[3]utt_f0_b1!H6</f>
-        <v>10.51</v>
+        <v>10.56</v>
       </c>
       <c r="I7" s="18">
         <f>[3]utt_f0_b1!I6</f>
-        <v>1.34E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="J7" s="40">
         <f>[3]utt_f0_b1!J6</f>
-        <v>1.89E-2</v>
-      </c>
-      <c r="K7" s="16" t="str">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K7" s="16">
         <f>[3]utt_f0_b1!K6</f>
-        <v>p&lt;0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4710,39 +4701,39 @@
       </c>
       <c r="C8" s="42">
         <f>[3]utt_f0_b1!C7</f>
-        <v>1.53</v>
+        <v>1.079</v>
       </c>
       <c r="D8" s="42">
         <f>[3]utt_f0_b1!D7</f>
-        <v>0.58799999999999997</v>
+        <v>-4.86078358637431E-2</v>
       </c>
       <c r="E8" s="42">
         <f>[3]utt_f0_b1!E7</f>
-        <v>0.377</v>
+        <v>2.2068583933924799</v>
       </c>
       <c r="F8" s="42">
         <f>[3]utt_f0_b1!F7</f>
-        <v>2.6829999999999998</v>
+        <v>0.50700000000000001</v>
       </c>
       <c r="G8" s="42">
         <f>[3]utt_f0_b1!G7</f>
-        <v>2.6019999999999999</v>
+        <v>2.1269999999999998</v>
       </c>
       <c r="H8" s="43">
         <f>[3]utt_f0_b1!H7</f>
-        <v>10.050000000000001</v>
+        <v>10.17</v>
       </c>
       <c r="I8" s="43">
         <f>[3]utt_f0_b1!I7</f>
-        <v>2.63E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="J8" s="44">
         <f>[3]utt_f0_b1!J7</f>
-        <v>3.32E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="K8" s="41" t="str">
         <f>[3]utt_f0_b1!K7</f>
-        <v>p&lt;0.05</v>
+        <v>(p&lt;0.1)</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4765,15 +4756,15 @@
       </c>
       <c r="D11" s="8" t="str">
         <f>[5]utt_slope_b1!D1</f>
-        <v>std.error</v>
+        <v>conf.low</v>
       </c>
       <c r="E11" s="8" t="str">
         <f>[5]utt_slope_b1!E1</f>
-        <v>2.5% CI</v>
+        <v>conf.high</v>
       </c>
       <c r="F11" s="8" t="str">
         <f>[5]utt_slope_b1!F1</f>
-        <v>97.5% CI</v>
+        <v>std.error</v>
       </c>
       <c r="G11" s="8" t="str">
         <f>[5]utt_slope_b1!G1</f>
@@ -4813,35 +4804,35 @@
       </c>
       <c r="C12" s="12">
         <f>[5]utt_slope_b1!C2</f>
-        <v>-2.028</v>
+        <v>-2.093</v>
       </c>
       <c r="D12" s="12">
         <f>[5]utt_slope_b1!D2</f>
-        <v>1.234</v>
+        <v>-4.8500048198338899</v>
       </c>
       <c r="E12" s="12">
         <f>[5]utt_slope_b1!E2</f>
-        <v>-4.4470000000000001</v>
+        <v>0.66381613021775598</v>
       </c>
       <c r="F12" s="12">
         <f>[5]utt_slope_b1!F2</f>
-        <v>0.39200000000000002</v>
+        <v>1.2390000000000001</v>
       </c>
       <c r="G12" s="12">
         <f>[5]utt_slope_b1!G2</f>
-        <v>-1.643</v>
+        <v>-1.6890000000000001</v>
       </c>
       <c r="H12" s="12">
         <f>[5]utt_slope_b1!H2</f>
-        <v>10.15</v>
+        <v>10.11</v>
       </c>
       <c r="I12" s="13">
         <f>[5]utt_slope_b1!I2</f>
-        <v>0.13100000000000001</v>
+        <v>0.122</v>
       </c>
       <c r="J12" s="14">
         <f>[5]utt_slope_b1!J2</f>
-        <v>0.14979999999999999</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="K12" s="11">
         <f>[5]utt_slope_b1!K2</f>
@@ -4849,11 +4840,11 @@
       </c>
       <c r="M12" s="39">
         <f>[6]utt_slope_r2!$B$3</f>
-        <v>0.51029969546325904</v>
+        <v>0.26953753570664701</v>
       </c>
       <c r="N12" s="39">
         <f>[6]utt_slope_r2!$B$2</f>
-        <v>0.83641134398527495</v>
+        <v>0.91258286194614602</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4867,35 +4858,35 @@
       </c>
       <c r="C13" s="17">
         <f>[5]utt_slope_b1!C3</f>
-        <v>3.3940000000000001</v>
+        <v>2.907</v>
       </c>
       <c r="D13" s="17">
         <f>[5]utt_slope_b1!D3</f>
-        <v>0.8</v>
+        <v>1.2891062804668101</v>
       </c>
       <c r="E13" s="17">
         <f>[5]utt_slope_b1!E3</f>
-        <v>1.825</v>
+        <v>4.5244332348265397</v>
       </c>
       <c r="F13" s="17">
         <f>[5]utt_slope_b1!F3</f>
-        <v>4.9630000000000001</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="G13" s="17">
         <f>[5]utt_slope_b1!G3</f>
-        <v>4.24</v>
+        <v>3.9969999999999999</v>
       </c>
       <c r="H13" s="45">
         <f>[5]utt_slope_b1!H3</f>
-        <v>10.02</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="I13" s="18">
         <f>[5]utt_slope_b1!I3</f>
-        <v>1.6999999999999999E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="J13" s="19">
         <f>[5]utt_slope_b1!J3</f>
-        <v>3.7000000000000002E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="K13" s="16" t="str">
         <f>[5]utt_slope_b1!K3</f>
@@ -4913,39 +4904,39 @@
       </c>
       <c r="C14" s="17">
         <f>[5]utt_slope_b1!C4</f>
-        <v>6.38</v>
+        <v>5.07</v>
       </c>
       <c r="D14" s="17">
         <f>[5]utt_slope_b1!D4</f>
-        <v>1.1180000000000001</v>
+        <v>3.0169488394014401</v>
       </c>
       <c r="E14" s="17">
         <f>[5]utt_slope_b1!E4</f>
-        <v>4.1890000000000001</v>
+        <v>7.1230429774581703</v>
       </c>
       <c r="F14" s="17">
         <f>[5]utt_slope_b1!F4</f>
-        <v>8.57</v>
+        <v>0.93</v>
       </c>
       <c r="G14" s="17">
         <f>[5]utt_slope_b1!G4</f>
-        <v>5.7089999999999996</v>
+        <v>5.4489999999999998</v>
       </c>
       <c r="H14" s="45">
         <f>[5]utt_slope_b1!H4</f>
-        <v>10.119999999999999</v>
+        <v>10.78</v>
       </c>
       <c r="I14" s="18">
         <f>[5]utt_slope_b1!I4</f>
-        <v>1.8699999999999999E-4</v>
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="J14" s="19">
         <f>[5]utt_slope_b1!J4</f>
-        <v>8.9999999999999998E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="K14" s="16" t="str">
         <f>[5]utt_slope_b1!K4</f>
-        <v>p&lt;0.001</v>
+        <v>p&lt;0.01</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4959,31 +4950,31 @@
       </c>
       <c r="C15" s="17">
         <f>[5]utt_slope_b1!C5</f>
-        <v>5.4219999999999997</v>
+        <v>5</v>
       </c>
       <c r="D15" s="17">
         <f>[5]utt_slope_b1!D5</f>
-        <v>1.4370000000000001</v>
+        <v>2.0744151301770501</v>
       </c>
       <c r="E15" s="17">
         <f>[5]utt_slope_b1!E5</f>
-        <v>2.6059999999999999</v>
+        <v>7.9253164313353501</v>
       </c>
       <c r="F15" s="17">
         <f>[5]utt_slope_b1!F5</f>
-        <v>8.2379999999999995</v>
+        <v>1.3169999999999999</v>
       </c>
       <c r="G15" s="17">
         <f>[5]utt_slope_b1!G5</f>
-        <v>3.7730000000000001</v>
+        <v>3.7959999999999998</v>
       </c>
       <c r="H15" s="45">
         <f>[5]utt_slope_b1!H5</f>
-        <v>10.26</v>
+        <v>10.24</v>
       </c>
       <c r="I15" s="18">
         <f>[5]utt_slope_b1!I5</f>
-        <v>3.5000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="J15" s="19">
         <f>[5]utt_slope_b1!J5</f>
@@ -5005,35 +4996,35 @@
       </c>
       <c r="C16" s="17">
         <f>[5]utt_slope_b1!C6</f>
-        <v>8.407</v>
+        <v>7.1630000000000003</v>
       </c>
       <c r="D16" s="17">
         <f>[5]utt_slope_b1!D6</f>
-        <v>1.796</v>
+        <v>3.63149587483408</v>
       </c>
       <c r="E16" s="17">
         <f>[5]utt_slope_b1!E6</f>
-        <v>4.8860000000000001</v>
+        <v>10.694690908964599</v>
       </c>
       <c r="F16" s="17">
         <f>[5]utt_slope_b1!F6</f>
-        <v>11.928000000000001</v>
+        <v>1.593</v>
       </c>
       <c r="G16" s="17">
         <f>[5]utt_slope_b1!G6</f>
-        <v>4.68</v>
+        <v>4.4950000000000001</v>
       </c>
       <c r="H16" s="45">
         <f>[5]utt_slope_b1!H6</f>
-        <v>10.199999999999999</v>
+        <v>10.41</v>
       </c>
       <c r="I16" s="18">
         <f>[5]utt_slope_b1!I6</f>
-        <v>8.2200000000000003E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="J16" s="19">
         <f>[5]utt_slope_b1!J6</f>
-        <v>2.2000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K16" s="16" t="str">
         <f>[5]utt_slope_b1!K6</f>
@@ -5051,39 +5042,39 @@
       </c>
       <c r="C17" s="42">
         <f>[5]utt_slope_b1!C7</f>
-        <v>2.9849999999999999</v>
+        <v>2.1629999999999998</v>
       </c>
       <c r="D17" s="42">
         <f>[5]utt_slope_b1!D7</f>
-        <v>0.876</v>
+        <v>0.87233269943435898</v>
       </c>
       <c r="E17" s="42">
         <f>[5]utt_slope_b1!E7</f>
-        <v>1.268</v>
+        <v>3.4541186027926698</v>
       </c>
       <c r="F17" s="42">
         <f>[5]utt_slope_b1!F7</f>
-        <v>4.7030000000000003</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="G17" s="42">
         <f>[5]utt_slope_b1!G7</f>
-        <v>3.4060000000000001</v>
+        <v>3.74</v>
       </c>
       <c r="H17" s="46">
         <f>[5]utt_slope_b1!H7</f>
-        <v>9.83</v>
+        <v>9.8699999999999992</v>
       </c>
       <c r="I17" s="43">
         <f>[5]utt_slope_b1!I7</f>
-        <v>6.8999999999999999E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J17" s="47">
         <f>[5]utt_slope_b1!J7</f>
-        <v>1.18E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="K17" s="41" t="str">
         <f>[5]utt_slope_b1!K7</f>
-        <v>p&lt;0.05</v>
+        <v>p&lt;0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>